<commit_message>
docs: Update documentation and tutorial notebooks.
Also:
- bump up minimum Python version to 3.11
</commit_message>
<xml_diff>
--- a/docs/_static/demo/demo_GHG_outputs_.xlsx
+++ b/docs/_static/demo/demo_GHG_outputs_.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="inputs" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="outputs" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="internals" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="inputs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="outputs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="internals" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -865,18 +865,18 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Yunzalin</t>
+          <t>Kabaung</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18.295</v>
+        <v>18.8967</v>
       </c>
       <c r="C2" t="n">
-        <v>97.3408</v>
+        <v>96.2208</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>35</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -885,40 +885,40 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>21.3</v>
+        <v>21.6</v>
       </c>
       <c r="G2" t="n">
-        <v>23.3</v>
+        <v>23.7</v>
       </c>
       <c r="H2" t="n">
-        <v>26.2</v>
+        <v>27.2</v>
       </c>
       <c r="I2" t="n">
-        <v>28.9</v>
+        <v>30.1</v>
       </c>
       <c r="J2" t="n">
-        <v>28.3</v>
+        <v>29.3</v>
       </c>
       <c r="K2" t="n">
-        <v>26.3</v>
+        <v>26.9</v>
       </c>
       <c r="L2" t="n">
-        <v>25.9</v>
+        <v>26.5</v>
       </c>
       <c r="M2" t="n">
-        <v>25.9</v>
+        <v>26.5</v>
       </c>
       <c r="N2" t="n">
-        <v>26.2</v>
+        <v>27</v>
       </c>
       <c r="O2" t="n">
-        <v>26.1</v>
+        <v>27.3</v>
       </c>
       <c r="P2" t="n">
-        <v>24.5</v>
+        <v>25.4</v>
       </c>
       <c r="Q2" t="n">
-        <v>21.9</v>
+        <v>22.3</v>
       </c>
       <c r="R2" t="n">
         <v>1</v>
@@ -966,16 +966,16 @@
         </is>
       </c>
       <c r="AE2" t="n">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AF2" t="n">
-        <v>1370.371</v>
+        <v>1181.378</v>
       </c>
       <c r="AG2" t="n">
-        <v>5.59</v>
+        <v>21.602</v>
       </c>
       <c r="AH2" t="n">
-        <v>3908</v>
+        <v>142154</v>
       </c>
       <c r="AI2" t="n">
         <v>0</v>
@@ -990,46 +990,46 @@
         <v>0</v>
       </c>
       <c r="AM2" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="AN2" t="n">
         <v>0.002</v>
       </c>
-      <c r="AN2" t="n">
-        <v>0.003</v>
-      </c>
       <c r="AO2" t="n">
-        <v>0.459</v>
+        <v>0.349</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.536</v>
+        <v>0.646</v>
       </c>
       <c r="AQ2" t="n">
         <v>0</v>
       </c>
       <c r="AR2" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="AS2" t="n">
-        <v>1451</v>
+        <v>1498</v>
       </c>
       <c r="AT2" t="n">
-        <v>1274</v>
+        <v>1346</v>
       </c>
       <c r="AU2" t="n">
-        <v>412</v>
+        <v>323</v>
       </c>
       <c r="AV2" t="n">
-        <v>5.658</v>
+        <v>5.231</v>
       </c>
       <c r="AW2" t="n">
-        <v>461865094</v>
+        <v>591966860</v>
       </c>
       <c r="AX2" t="n">
-        <v>6.791</v>
+        <v>44.194</v>
       </c>
       <c r="AY2" t="n">
-        <v>185</v>
+        <v>39</v>
       </c>
       <c r="AZ2" t="n">
-        <v>68</v>
+        <v>13.4</v>
       </c>
       <c r="BA2" t="n">
         <v>0</v>
@@ -1044,16 +1044,16 @@
         <v>0</v>
       </c>
       <c r="BE2" t="n">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="BF2" t="n">
-        <v>0</v>
+        <v>0.031</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.97</v>
+        <v>0.755</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.03</v>
+        <v>0.139</v>
       </c>
       <c r="BI2" t="n">
         <v>0</v>
@@ -1113,37 +1113,37 @@
         <v>0</v>
       </c>
       <c r="CB2" t="n">
-        <v>5.648</v>
+        <v>5.021</v>
       </c>
       <c r="CC2" t="n">
-        <v>4.92</v>
+        <v>5.03</v>
       </c>
       <c r="CD2" t="n">
-        <v>4.17</v>
+        <v>4.34</v>
       </c>
       <c r="CE2" t="n">
-        <v>5.416</v>
+        <v>5.458</v>
       </c>
       <c r="CF2" t="n">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="CG2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Belin</t>
+          <t>Kun Chaung</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17.5197</v>
+        <v>18.4204</v>
       </c>
       <c r="C3" t="n">
-        <v>97.2435</v>
+        <v>96.3639</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>47</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1152,28 +1152,28 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>22.3</v>
+        <v>21.6</v>
       </c>
       <c r="G3" t="n">
-        <v>24</v>
+        <v>23.6</v>
       </c>
       <c r="H3" t="n">
-        <v>27</v>
+        <v>26.9</v>
       </c>
       <c r="I3" t="n">
-        <v>29.5</v>
+        <v>29.7</v>
       </c>
       <c r="J3" t="n">
-        <v>28.9</v>
+        <v>29</v>
       </c>
       <c r="K3" t="n">
-        <v>26.8</v>
+        <v>26.7</v>
       </c>
       <c r="L3" t="n">
-        <v>26.3</v>
+        <v>26.2</v>
       </c>
       <c r="M3" t="n">
-        <v>26.3</v>
+        <v>26.2</v>
       </c>
       <c r="N3" t="n">
         <v>26.8</v>
@@ -1182,10 +1182,10 @@
         <v>27.1</v>
       </c>
       <c r="P3" t="n">
-        <v>25.7</v>
+        <v>25.3</v>
       </c>
       <c r="Q3" t="n">
-        <v>23.1</v>
+        <v>22.3</v>
       </c>
       <c r="R3" t="n">
         <v>1</v>
@@ -1233,16 +1233,16 @@
         </is>
       </c>
       <c r="AE3" t="n">
-        <v>1578</v>
+        <v>833</v>
       </c>
       <c r="AF3" t="n">
-        <v>1906.529</v>
+        <v>871.239</v>
       </c>
       <c r="AG3" t="n">
-        <v>74.985</v>
+        <v>24.482</v>
       </c>
       <c r="AH3" t="n">
-        <v>12238</v>
+        <v>80370</v>
       </c>
       <c r="AI3" t="n">
         <v>0</v>
@@ -1257,46 +1257,46 @@
         <v>0</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.028</v>
+        <v>0.049</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.671</v>
+        <v>0.337</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.284</v>
+        <v>0.594</v>
       </c>
       <c r="AQ3" t="n">
         <v>0</v>
       </c>
       <c r="AR3" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="AS3" t="n">
-        <v>2619</v>
+        <v>1852</v>
       </c>
       <c r="AT3" t="n">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="AU3" t="n">
-        <v>527</v>
+        <v>366</v>
       </c>
       <c r="AV3" t="n">
-        <v>7.322</v>
+        <v>5.291</v>
       </c>
       <c r="AW3" t="n">
-        <v>26052597058</v>
+        <v>833157705</v>
       </c>
       <c r="AX3" t="n">
-        <v>434.864</v>
+        <v>65.65000000000001</v>
       </c>
       <c r="AY3" t="n">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="AZ3" t="n">
-        <v>59.9</v>
+        <v>12.7</v>
       </c>
       <c r="BA3" t="n">
         <v>0</v>
@@ -1311,16 +1311,16 @@
         <v>0</v>
       </c>
       <c r="BE3" t="n">
-        <v>0</v>
+        <v>0.583</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.075</v>
+        <v>0.172</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.776</v>
+        <v>0.157</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.149</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="BI3" t="n">
         <v>0</v>
@@ -1380,37 +1380,37 @@
         <v>0</v>
       </c>
       <c r="CB3" t="n">
-        <v>6.04</v>
+        <v>4.96</v>
       </c>
       <c r="CC3" t="n">
-        <v>4.87</v>
+        <v>5.03</v>
       </c>
       <c r="CD3" t="n">
-        <v>3.995</v>
+        <v>4.34</v>
       </c>
       <c r="CE3" t="n">
-        <v>5.459</v>
+        <v>5.458</v>
       </c>
       <c r="CF3" t="n">
-        <v>1.05</v>
+        <v>0.96</v>
       </c>
       <c r="CG3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Kabaung</t>
+          <t>Thauk Ye Khat 2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>18.8967</v>
+        <v>18.9141</v>
       </c>
       <c r="C4" t="n">
-        <v>96.2208</v>
+        <v>96.6199</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>120</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1419,25 +1419,25 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>21.6</v>
+        <v>21.9</v>
       </c>
       <c r="G4" t="n">
-        <v>23.7</v>
+        <v>24.2</v>
       </c>
       <c r="H4" t="n">
-        <v>27.2</v>
+        <v>27.5</v>
       </c>
       <c r="I4" t="n">
-        <v>30.1</v>
+        <v>30.3</v>
       </c>
       <c r="J4" t="n">
-        <v>29.3</v>
+        <v>29.2</v>
       </c>
       <c r="K4" t="n">
-        <v>26.9</v>
+        <v>27</v>
       </c>
       <c r="L4" t="n">
-        <v>26.5</v>
+        <v>26.6</v>
       </c>
       <c r="M4" t="n">
         <v>26.5</v>
@@ -1449,10 +1449,10 @@
         <v>27.3</v>
       </c>
       <c r="P4" t="n">
-        <v>25.4</v>
+        <v>25.5</v>
       </c>
       <c r="Q4" t="n">
-        <v>22.3</v>
+        <v>22.5</v>
       </c>
       <c r="R4" t="n">
         <v>1</v>
@@ -1500,16 +1500,16 @@
         </is>
       </c>
       <c r="AE4" t="n">
-        <v>470</v>
+        <v>447</v>
       </c>
       <c r="AF4" t="n">
-        <v>1181.378</v>
+        <v>2160.344</v>
       </c>
       <c r="AG4" t="n">
-        <v>21.602</v>
+        <v>12.272</v>
       </c>
       <c r="AH4" t="n">
-        <v>142154</v>
+        <v>56447</v>
       </c>
       <c r="AI4" t="n">
         <v>0</v>
@@ -1524,46 +1524,46 @@
         <v>0</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.349</v>
+        <v>0.436</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.646</v>
+        <v>0.554</v>
       </c>
       <c r="AQ4" t="n">
         <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="AS4" t="n">
-        <v>1498</v>
+        <v>1476</v>
       </c>
       <c r="AT4" t="n">
-        <v>1346</v>
+        <v>1325</v>
       </c>
       <c r="AU4" t="n">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="AV4" t="n">
-        <v>5.231</v>
+        <v>7.836</v>
       </c>
       <c r="AW4" t="n">
-        <v>591966860</v>
+        <v>171838645</v>
       </c>
       <c r="AX4" t="n">
-        <v>44.194</v>
+        <v>8.609999999999999</v>
       </c>
       <c r="AY4" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="AZ4" t="n">
-        <v>13.4</v>
+        <v>20</v>
       </c>
       <c r="BA4" t="n">
         <v>0</v>
@@ -1578,16 +1578,16 @@
         <v>0</v>
       </c>
       <c r="BE4" t="n">
-        <v>0.075</v>
+        <v>0.177</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.031</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.755</v>
+        <v>0.042</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.139</v>
+        <v>0.094</v>
       </c>
       <c r="BI4" t="n">
         <v>0</v>
@@ -1647,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="CB4" t="n">
-        <v>5.021</v>
+        <v>5.243</v>
       </c>
       <c r="CC4" t="n">
         <v>5.03</v>
@@ -1659,25 +1659,25 @@
         <v>5.458</v>
       </c>
       <c r="CF4" t="n">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="CG4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Kun Chaung</t>
+          <t>Phyu Chaung</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18.4204</v>
+        <v>18.5067</v>
       </c>
       <c r="C5" t="n">
-        <v>96.3639</v>
+        <v>96.3519</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>101</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1686,22 +1686,22 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>21.6</v>
+        <v>21.3</v>
       </c>
       <c r="G5" t="n">
-        <v>23.6</v>
+        <v>23.5</v>
       </c>
       <c r="H5" t="n">
         <v>26.9</v>
       </c>
       <c r="I5" t="n">
-        <v>29.7</v>
+        <v>29.9</v>
       </c>
       <c r="J5" t="n">
         <v>29</v>
       </c>
       <c r="K5" t="n">
-        <v>26.7</v>
+        <v>26.6</v>
       </c>
       <c r="L5" t="n">
         <v>26.2</v>
@@ -1710,16 +1710,16 @@
         <v>26.2</v>
       </c>
       <c r="N5" t="n">
-        <v>26.8</v>
+        <v>26.7</v>
       </c>
       <c r="O5" t="n">
-        <v>27.1</v>
+        <v>27</v>
       </c>
       <c r="P5" t="n">
-        <v>25.3</v>
+        <v>25.2</v>
       </c>
       <c r="Q5" t="n">
-        <v>22.3</v>
+        <v>22.1</v>
       </c>
       <c r="R5" t="n">
         <v>1</v>
@@ -1767,16 +1767,16 @@
         </is>
       </c>
       <c r="AE5" t="n">
-        <v>833</v>
+        <v>677</v>
       </c>
       <c r="AF5" t="n">
-        <v>871.239</v>
+        <v>1041.477</v>
       </c>
       <c r="AG5" t="n">
-        <v>24.482</v>
+        <v>30.545</v>
       </c>
       <c r="AH5" t="n">
-        <v>80370</v>
+        <v>106274</v>
       </c>
       <c r="AI5" t="n">
         <v>0</v>
@@ -1791,16 +1791,16 @@
         <v>0</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.049</v>
+        <v>0.026</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.02</v>
+        <v>0.004</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.337</v>
+        <v>0.39</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.594</v>
+        <v>0.58</v>
       </c>
       <c r="AQ5" t="n">
         <v>0</v>
@@ -1809,28 +1809,28 @@
         <v>11</v>
       </c>
       <c r="AS5" t="n">
-        <v>1852</v>
+        <v>1707</v>
       </c>
       <c r="AT5" t="n">
-        <v>1337</v>
+        <v>1341</v>
       </c>
       <c r="AU5" t="n">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="AV5" t="n">
-        <v>5.291</v>
+        <v>4.881</v>
       </c>
       <c r="AW5" t="n">
-        <v>833157705</v>
+        <v>540574414</v>
       </c>
       <c r="AX5" t="n">
-        <v>65.65000000000001</v>
+        <v>42.19</v>
       </c>
       <c r="AY5" t="n">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="AZ5" t="n">
-        <v>12.7</v>
+        <v>12.8</v>
       </c>
       <c r="BA5" t="n">
         <v>0</v>
@@ -1845,16 +1845,16 @@
         <v>0</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.583</v>
+        <v>0.55</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.172</v>
+        <v>0.052</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.157</v>
+        <v>0.12</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.278</v>
       </c>
       <c r="BI5" t="n">
         <v>0</v>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="CB5" t="n">
-        <v>4.96</v>
+        <v>5.068</v>
       </c>
       <c r="CC5" t="n">
         <v>5.03</v>
@@ -1926,25 +1926,25 @@
         <v>5.458</v>
       </c>
       <c r="CF5" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
       <c r="CG5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Thauk Ye Khat 2</t>
+          <t>Shwegyin</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18.9141</v>
+        <v>17.9702</v>
       </c>
       <c r="C6" t="n">
-        <v>96.6199</v>
+        <v>96.935</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>107</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1953,40 +1953,40 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>21.9</v>
+        <v>22.9</v>
       </c>
       <c r="G6" t="n">
-        <v>24.2</v>
+        <v>24.7</v>
       </c>
       <c r="H6" t="n">
-        <v>27.5</v>
+        <v>27.7</v>
       </c>
       <c r="I6" t="n">
-        <v>30.3</v>
+        <v>30.2</v>
       </c>
       <c r="J6" t="n">
-        <v>29.2</v>
+        <v>29.5</v>
       </c>
       <c r="K6" t="n">
-        <v>27</v>
+        <v>27.3</v>
       </c>
       <c r="L6" t="n">
-        <v>26.6</v>
+        <v>26.9</v>
       </c>
       <c r="M6" t="n">
-        <v>26.5</v>
+        <v>26.8</v>
       </c>
       <c r="N6" t="n">
-        <v>27</v>
+        <v>27.3</v>
       </c>
       <c r="O6" t="n">
-        <v>27.3</v>
+        <v>27.6</v>
       </c>
       <c r="P6" t="n">
-        <v>25.5</v>
+        <v>26.2</v>
       </c>
       <c r="Q6" t="n">
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="R6" t="n">
         <v>1</v>
@@ -2034,16 +2034,16 @@
         </is>
       </c>
       <c r="AE6" t="n">
-        <v>447</v>
+        <v>1423</v>
       </c>
       <c r="AF6" t="n">
-        <v>2160.344</v>
+        <v>874.105</v>
       </c>
       <c r="AG6" t="n">
-        <v>12.272</v>
+        <v>30.778</v>
       </c>
       <c r="AH6" t="n">
-        <v>56447</v>
+        <v>36013</v>
       </c>
       <c r="AI6" t="n">
         <v>0</v>
@@ -2058,46 +2058,46 @@
         <v>0</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.004</v>
+        <v>0.056</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.005</v>
+        <v>0.023</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.436</v>
+        <v>0.392</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.554</v>
+        <v>0.528</v>
       </c>
       <c r="AQ6" t="n">
         <v>0</v>
       </c>
       <c r="AR6" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AS6" t="n">
-        <v>1476</v>
+        <v>2449</v>
       </c>
       <c r="AT6" t="n">
-        <v>1325</v>
+        <v>1320</v>
       </c>
       <c r="AU6" t="n">
-        <v>343</v>
+        <v>501</v>
       </c>
       <c r="AV6" t="n">
-        <v>7.836</v>
+        <v>9.629</v>
       </c>
       <c r="AW6" t="n">
-        <v>171838645</v>
+        <v>1725920668</v>
       </c>
       <c r="AX6" t="n">
-        <v>8.609999999999999</v>
+        <v>86.029</v>
       </c>
       <c r="AY6" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="AZ6" t="n">
-        <v>20</v>
+        <v>20.1</v>
       </c>
       <c r="BA6" t="n">
         <v>0</v>
@@ -2112,16 +2112,16 @@
         <v>0</v>
       </c>
       <c r="BE6" t="n">
-        <v>0.177</v>
+        <v>0.462</v>
       </c>
       <c r="BF6" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.215</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.042</v>
+        <v>0.096</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.094</v>
+        <v>0.227</v>
       </c>
       <c r="BI6" t="n">
         <v>0</v>
@@ -2181,37 +2181,37 @@
         <v>0</v>
       </c>
       <c r="CB6" t="n">
-        <v>5.243</v>
+        <v>6.145</v>
       </c>
       <c r="CC6" t="n">
-        <v>5.03</v>
+        <v>4.94</v>
       </c>
       <c r="CD6" t="n">
-        <v>4.34</v>
+        <v>4.16</v>
       </c>
       <c r="CE6" t="n">
-        <v>5.458</v>
+        <v>5.445</v>
       </c>
       <c r="CF6" t="n">
-        <v>1.05</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="CG6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Phyu Chaung</t>
+          <t>Belin</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18.5067</v>
+        <v>17.5197</v>
       </c>
       <c r="C7" t="n">
-        <v>96.3519</v>
+        <v>97.2435</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2220,40 +2220,40 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>21.3</v>
+        <v>22.3</v>
       </c>
       <c r="G7" t="n">
-        <v>23.5</v>
+        <v>24</v>
       </c>
       <c r="H7" t="n">
-        <v>26.9</v>
+        <v>27</v>
       </c>
       <c r="I7" t="n">
-        <v>29.9</v>
+        <v>29.5</v>
       </c>
       <c r="J7" t="n">
-        <v>29</v>
+        <v>28.9</v>
       </c>
       <c r="K7" t="n">
-        <v>26.6</v>
+        <v>26.8</v>
       </c>
       <c r="L7" t="n">
-        <v>26.2</v>
+        <v>26.3</v>
       </c>
       <c r="M7" t="n">
-        <v>26.2</v>
+        <v>26.3</v>
       </c>
       <c r="N7" t="n">
-        <v>26.7</v>
+        <v>26.8</v>
       </c>
       <c r="O7" t="n">
-        <v>27</v>
+        <v>27.1</v>
       </c>
       <c r="P7" t="n">
-        <v>25.2</v>
+        <v>25.7</v>
       </c>
       <c r="Q7" t="n">
-        <v>22.1</v>
+        <v>23.1</v>
       </c>
       <c r="R7" t="n">
         <v>1</v>
@@ -2301,16 +2301,16 @@
         </is>
       </c>
       <c r="AE7" t="n">
-        <v>677</v>
+        <v>1578</v>
       </c>
       <c r="AF7" t="n">
-        <v>1041.477</v>
+        <v>1906.529</v>
       </c>
       <c r="AG7" t="n">
-        <v>30.545</v>
+        <v>74.985</v>
       </c>
       <c r="AH7" t="n">
-        <v>106274</v>
+        <v>12238</v>
       </c>
       <c r="AI7" t="n">
         <v>0</v>
@@ -2325,46 +2325,46 @@
         <v>0</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.026</v>
+        <v>0.028</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.004</v>
+        <v>0.018</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.39</v>
+        <v>0.671</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.58</v>
+        <v>0.284</v>
       </c>
       <c r="AQ7" t="n">
         <v>0</v>
       </c>
       <c r="AR7" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="AS7" t="n">
-        <v>1707</v>
+        <v>2619</v>
       </c>
       <c r="AT7" t="n">
-        <v>1341</v>
+        <v>1338</v>
       </c>
       <c r="AU7" t="n">
-        <v>355</v>
+        <v>527</v>
       </c>
       <c r="AV7" t="n">
-        <v>4.881</v>
+        <v>7.322</v>
       </c>
       <c r="AW7" t="n">
-        <v>540574414</v>
+        <v>26052597058</v>
       </c>
       <c r="AX7" t="n">
-        <v>42.19</v>
+        <v>434.864</v>
       </c>
       <c r="AY7" t="n">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="AZ7" t="n">
-        <v>12.8</v>
+        <v>59.9</v>
       </c>
       <c r="BA7" t="n">
         <v>0</v>
@@ -2379,16 +2379,16 @@
         <v>0</v>
       </c>
       <c r="BE7" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
       <c r="BF7" t="n">
-        <v>0.052</v>
+        <v>0.075</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.12</v>
+        <v>0.776</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.278</v>
+        <v>0.149</v>
       </c>
       <c r="BI7" t="n">
         <v>0</v>
@@ -2448,37 +2448,37 @@
         <v>0</v>
       </c>
       <c r="CB7" t="n">
-        <v>5.068</v>
+        <v>6.04</v>
       </c>
       <c r="CC7" t="n">
-        <v>5.03</v>
+        <v>4.87</v>
       </c>
       <c r="CD7" t="n">
-        <v>4.34</v>
+        <v>3.995</v>
       </c>
       <c r="CE7" t="n">
-        <v>5.458</v>
+        <v>5.459</v>
       </c>
       <c r="CF7" t="n">
-        <v>0.99</v>
+        <v>1.05</v>
       </c>
       <c r="CG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Shwegyin</t>
+          <t>Yunzalin</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17.9702</v>
+        <v>18.295</v>
       </c>
       <c r="C8" t="n">
-        <v>96.935</v>
+        <v>97.3408</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>152</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2487,40 +2487,40 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>22.9</v>
+        <v>21.3</v>
       </c>
       <c r="G8" t="n">
-        <v>24.7</v>
+        <v>23.3</v>
       </c>
       <c r="H8" t="n">
-        <v>27.7</v>
+        <v>26.2</v>
       </c>
       <c r="I8" t="n">
-        <v>30.2</v>
+        <v>28.9</v>
       </c>
       <c r="J8" t="n">
-        <v>29.5</v>
+        <v>28.3</v>
       </c>
       <c r="K8" t="n">
-        <v>27.3</v>
+        <v>26.3</v>
       </c>
       <c r="L8" t="n">
-        <v>26.9</v>
+        <v>25.9</v>
       </c>
       <c r="M8" t="n">
-        <v>26.8</v>
+        <v>25.9</v>
       </c>
       <c r="N8" t="n">
-        <v>27.3</v>
+        <v>26.2</v>
       </c>
       <c r="O8" t="n">
-        <v>27.6</v>
+        <v>26.1</v>
       </c>
       <c r="P8" t="n">
-        <v>26.2</v>
+        <v>24.5</v>
       </c>
       <c r="Q8" t="n">
-        <v>23.5</v>
+        <v>21.9</v>
       </c>
       <c r="R8" t="n">
         <v>1</v>
@@ -2568,16 +2568,16 @@
         </is>
       </c>
       <c r="AE8" t="n">
-        <v>1423</v>
+        <v>469</v>
       </c>
       <c r="AF8" t="n">
-        <v>874.105</v>
+        <v>1370.371</v>
       </c>
       <c r="AG8" t="n">
-        <v>30.778</v>
+        <v>5.59</v>
       </c>
       <c r="AH8" t="n">
-        <v>36013</v>
+        <v>3908</v>
       </c>
       <c r="AI8" t="n">
         <v>0</v>
@@ -2592,16 +2592,16 @@
         <v>0</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.056</v>
+        <v>0.002</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.023</v>
+        <v>0.003</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.392</v>
+        <v>0.459</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.528</v>
+        <v>0.536</v>
       </c>
       <c r="AQ8" t="n">
         <v>0</v>
@@ -2610,28 +2610,28 @@
         <v>24</v>
       </c>
       <c r="AS8" t="n">
-        <v>2449</v>
+        <v>1451</v>
       </c>
       <c r="AT8" t="n">
-        <v>1320</v>
+        <v>1274</v>
       </c>
       <c r="AU8" t="n">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="AV8" t="n">
-        <v>9.629</v>
+        <v>5.658</v>
       </c>
       <c r="AW8" t="n">
-        <v>1725920668</v>
+        <v>461865094</v>
       </c>
       <c r="AX8" t="n">
-        <v>86.029</v>
+        <v>6.791</v>
       </c>
       <c r="AY8" t="n">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="AZ8" t="n">
-        <v>20.1</v>
+        <v>68</v>
       </c>
       <c r="BA8" t="n">
         <v>0</v>
@@ -2646,16 +2646,16 @@
         <v>0</v>
       </c>
       <c r="BE8" t="n">
-        <v>0.462</v>
+        <v>0</v>
       </c>
       <c r="BF8" t="n">
-        <v>0.215</v>
+        <v>0</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.096</v>
+        <v>0.97</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.227</v>
+        <v>0.03</v>
       </c>
       <c r="BI8" t="n">
         <v>0</v>
@@ -2715,19 +2715,19 @@
         <v>0</v>
       </c>
       <c r="CB8" t="n">
-        <v>6.145</v>
+        <v>5.648</v>
       </c>
       <c r="CC8" t="n">
-        <v>4.94</v>
+        <v>4.92</v>
       </c>
       <c r="CD8" t="n">
-        <v>4.16</v>
+        <v>4.17</v>
       </c>
       <c r="CE8" t="n">
-        <v>5.445</v>
+        <v>5.416</v>
       </c>
       <c r="CF8" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.04</v>
       </c>
       <c r="CG8" t="inlineStr"/>
     </row>
@@ -4073,1079 +4073,1079 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Yunzalin</t>
+          <t>Kabaung</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>614.0891</v>
+        <v>1067.8172</v>
       </c>
       <c r="C2" t="n">
-        <v>421.4361</v>
+        <v>732.9157</v>
       </c>
       <c r="D2" t="n">
-        <v>-15.4</v>
+        <v>-71.3533</v>
       </c>
       <c r="E2" t="n">
-        <v>192.653</v>
+        <v>334.9014</v>
       </c>
       <c r="F2" t="n">
-        <v>208.053</v>
+        <v>406.2548</v>
       </c>
       <c r="G2" t="n">
-        <v>1412.8879</v>
+        <v>17954.023</v>
       </c>
       <c r="H2" t="n">
-        <v>141.2888</v>
+        <v>1795.4023</v>
       </c>
       <c r="I2" t="n">
-        <v>1520.2986</v>
+        <v>2688.5089</v>
       </c>
       <c r="J2" t="n">
-        <v>726.5511</v>
+        <v>1308.1097</v>
       </c>
       <c r="K2" t="n">
-        <v>494.9783</v>
+        <v>905.3837</v>
       </c>
       <c r="L2" t="n">
-        <v>310.7537</v>
+        <v>585.0004</v>
       </c>
       <c r="M2" t="n">
-        <v>220.9844</v>
+        <v>428.8833</v>
       </c>
       <c r="N2" t="n">
-        <v>164.1964</v>
+        <v>330.1237</v>
       </c>
       <c r="O2" t="n">
-        <v>123.7147</v>
+        <v>259.7225</v>
       </c>
       <c r="P2" t="n">
-        <v>79.7782</v>
+        <v>183.3129</v>
       </c>
       <c r="Q2" t="n">
-        <v>47.6046</v>
+        <v>127.3601</v>
       </c>
       <c r="R2" t="n">
-        <v>15.4</v>
+        <v>71.3533</v>
       </c>
       <c r="S2" t="n">
-        <v>99.7324</v>
+        <v>238.6546</v>
       </c>
       <c r="T2" t="n">
-        <v>44.8219</v>
+        <v>210.6076</v>
       </c>
       <c r="U2" t="n">
-        <v>306.4067</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>450.9609</v>
+        <v>449.2623</v>
       </c>
       <c r="X2" t="n">
-        <v>3062.4757</v>
+        <v>19854.6961</v>
       </c>
       <c r="Y2" t="n">
-        <v>306.2476</v>
+        <v>1985.4696</v>
       </c>
       <c r="Z2" t="n">
-        <v>1390.7628</v>
+        <v>995.2125</v>
       </c>
       <c r="AA2" t="n">
-        <v>1225.8901</v>
+        <v>899.0871</v>
       </c>
       <c r="AB2" t="n">
-        <v>1047.9033</v>
+        <v>795.3183</v>
       </c>
       <c r="AC2" t="n">
-        <v>768.3554</v>
+        <v>632.3439</v>
       </c>
       <c r="AD2" t="n">
-        <v>566.7145</v>
+        <v>514.7949</v>
       </c>
       <c r="AE2" t="n">
-        <v>421.2687</v>
+        <v>430.0098</v>
       </c>
       <c r="AF2" t="n">
-        <v>316.357</v>
+        <v>368.8566</v>
       </c>
       <c r="AG2" t="n">
-        <v>211.1669</v>
+        <v>307.5449</v>
       </c>
       <c r="AH2" t="n">
-        <v>146.7264</v>
+        <v>269.9877</v>
       </c>
       <c r="AI2" t="n">
-        <v>97.8417</v>
+        <v>241.4993</v>
       </c>
       <c r="AJ2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AK2" t="n">
-        <v>1.6008</v>
+        <v>1.4976</v>
       </c>
       <c r="AL2" t="n">
-        <v>2.2033</v>
+        <v>2.4688</v>
       </c>
       <c r="AM2" t="n">
-        <v>19.0548</v>
+        <v>152.0319</v>
       </c>
       <c r="AN2" t="n">
-        <v>1.9055</v>
+        <v>15.2032</v>
       </c>
       <c r="AO2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AP2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AQ2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AR2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AS2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AT2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AU2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AV2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AW2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
       <c r="AX2" t="n">
-        <v>2.8059</v>
+        <v>3.4401</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Belin</t>
+          <t>Kun Chaung</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>541.4894</v>
+        <v>911.8052</v>
       </c>
       <c r="C3" t="n">
-        <v>371.6125</v>
+        <v>625.8341</v>
       </c>
       <c r="D3" t="n">
-        <v>-76.4867</v>
+        <v>-45.1733</v>
       </c>
       <c r="E3" t="n">
-        <v>169.8769</v>
+        <v>285.9711</v>
       </c>
       <c r="F3" t="n">
-        <v>246.3636</v>
+        <v>331.1445</v>
       </c>
       <c r="G3" t="n">
-        <v>107134.6446</v>
+        <v>21739.6337</v>
       </c>
       <c r="H3" t="n">
-        <v>10713.4645</v>
+        <v>2173.9634</v>
       </c>
       <c r="I3" t="n">
-        <v>1403.471</v>
+        <v>2279.953</v>
       </c>
       <c r="J3" t="n">
-        <v>703.563</v>
+        <v>1101.2352</v>
       </c>
       <c r="K3" t="n">
-        <v>499.3676</v>
+        <v>757.3488</v>
       </c>
       <c r="L3" t="n">
-        <v>336.9227</v>
+        <v>483.7747</v>
       </c>
       <c r="M3" t="n">
-        <v>257.7662</v>
+        <v>350.4669</v>
       </c>
       <c r="N3" t="n">
-        <v>207.6918</v>
+        <v>266.1365</v>
       </c>
       <c r="O3" t="n">
-        <v>171.996</v>
+        <v>206.0211</v>
       </c>
       <c r="P3" t="n">
-        <v>133.2539</v>
+        <v>140.7752</v>
       </c>
       <c r="Q3" t="n">
-        <v>104.884</v>
+        <v>92.9973</v>
       </c>
       <c r="R3" t="n">
-        <v>76.4867</v>
+        <v>45.1733</v>
       </c>
       <c r="S3" t="n">
-        <v>109.1442</v>
+        <v>244.8448</v>
       </c>
       <c r="T3" t="n">
-        <v>42.5642</v>
+        <v>231.526</v>
       </c>
       <c r="U3" t="n">
-        <v>130.6735</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>282.3818</v>
+        <v>476.3708</v>
       </c>
       <c r="X3" t="n">
-        <v>122797.6666</v>
+        <v>31273.7416</v>
       </c>
       <c r="Y3" t="n">
-        <v>12279.7667</v>
+        <v>3127.3742</v>
       </c>
       <c r="Z3" t="n">
-        <v>842.8341</v>
+        <v>1036.4817</v>
       </c>
       <c r="AA3" t="n">
-        <v>744.7999</v>
+        <v>937.8631</v>
       </c>
       <c r="AB3" t="n">
-        <v>638.9688</v>
+        <v>831.4027</v>
       </c>
       <c r="AC3" t="n">
-        <v>472.751</v>
+        <v>664.2012</v>
       </c>
       <c r="AD3" t="n">
-        <v>352.858</v>
+        <v>543.6032</v>
       </c>
       <c r="AE3" t="n">
-        <v>266.3792</v>
+        <v>456.619</v>
       </c>
       <c r="AF3" t="n">
-        <v>204.002</v>
+        <v>393.8796</v>
       </c>
       <c r="AG3" t="n">
-        <v>141.4603</v>
+        <v>330.9776</v>
       </c>
       <c r="AH3" t="n">
-        <v>103.1476</v>
+        <v>292.4463</v>
       </c>
       <c r="AI3" t="n">
-        <v>74.08410000000001</v>
+        <v>263.2189</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.1043</v>
+        <v>1.3163</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.3058</v>
+        <v>2.2593</v>
       </c>
       <c r="AM3" t="n">
-        <v>220.6093</v>
+        <v>210.2304</v>
       </c>
       <c r="AN3" t="n">
-        <v>22.0609</v>
+        <v>21.023</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.5073</v>
+        <v>3.2023</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Kabaung</t>
+          <t>Thauk Ye Khat 2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1067.9568</v>
+        <v>783.2979</v>
       </c>
       <c r="C4" t="n">
-        <v>732.9157</v>
+        <v>537.6308</v>
       </c>
       <c r="D4" t="n">
-        <v>-71.3533</v>
+        <v>-48.2533</v>
       </c>
       <c r="E4" t="n">
-        <v>335.0411</v>
+        <v>245.6671</v>
       </c>
       <c r="F4" t="n">
-        <v>406.3944</v>
+        <v>293.9205</v>
       </c>
       <c r="G4" t="n">
-        <v>17960.1948</v>
+        <v>2530.6553</v>
       </c>
       <c r="H4" t="n">
-        <v>1796.0195</v>
+        <v>253.0655</v>
       </c>
       <c r="I4" t="n">
-        <v>2688.5089</v>
+        <v>1968.0693</v>
       </c>
       <c r="J4" t="n">
-        <v>1308.1097</v>
+        <v>955.4767000000001</v>
       </c>
       <c r="K4" t="n">
-        <v>905.3837</v>
+        <v>660.0568</v>
       </c>
       <c r="L4" t="n">
-        <v>585.0004</v>
+        <v>425.0394</v>
       </c>
       <c r="M4" t="n">
-        <v>428.8833</v>
+        <v>310.5196</v>
       </c>
       <c r="N4" t="n">
-        <v>330.1237</v>
+        <v>238.0745</v>
       </c>
       <c r="O4" t="n">
-        <v>259.7225</v>
+        <v>186.4316</v>
       </c>
       <c r="P4" t="n">
-        <v>183.3129</v>
+        <v>130.3814</v>
       </c>
       <c r="Q4" t="n">
-        <v>127.3601</v>
+        <v>89.33710000000001</v>
       </c>
       <c r="R4" t="n">
-        <v>71.3533</v>
+        <v>48.2533</v>
       </c>
       <c r="S4" t="n">
-        <v>230.9829</v>
+        <v>190.1026</v>
       </c>
       <c r="T4" t="n">
-        <v>210.6076</v>
+        <v>134.7671</v>
       </c>
       <c r="U4" t="n">
-        <v>614.3304000000001</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>1055.921</v>
+        <v>324.8697</v>
       </c>
       <c r="X4" t="n">
-        <v>46665.372</v>
+        <v>2797.1278</v>
       </c>
       <c r="Y4" t="n">
-        <v>4666.5372</v>
+        <v>279.7128</v>
       </c>
       <c r="Z4" t="n">
-        <v>3014.5375</v>
+        <v>759.7514</v>
       </c>
       <c r="AA4" t="n">
-        <v>2671.0647</v>
+        <v>683.1818</v>
       </c>
       <c r="AB4" t="n">
-        <v>2300.2723</v>
+        <v>600.5238000000001</v>
       </c>
       <c r="AC4" t="n">
-        <v>1717.9024</v>
+        <v>470.7051</v>
       </c>
       <c r="AD4" t="n">
-        <v>1297.8336</v>
+        <v>377.0703</v>
       </c>
       <c r="AE4" t="n">
-        <v>994.8339</v>
+        <v>309.534</v>
       </c>
       <c r="AF4" t="n">
-        <v>776.2775</v>
+        <v>260.8218</v>
       </c>
       <c r="AG4" t="n">
-        <v>557.1413</v>
+        <v>211.9834</v>
       </c>
       <c r="AH4" t="n">
-        <v>422.8968</v>
+        <v>182.0669</v>
       </c>
       <c r="AI4" t="n">
-        <v>321.059</v>
+        <v>159.3741</v>
       </c>
       <c r="AJ4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AK4" t="n">
-        <v>1.4976</v>
+        <v>0.2595</v>
       </c>
       <c r="AL4" t="n">
-        <v>2.4688</v>
+        <v>0.294</v>
       </c>
       <c r="AM4" t="n">
-        <v>152.0319</v>
+        <v>2.8289</v>
       </c>
       <c r="AN4" t="n">
-        <v>15.2032</v>
+        <v>0.2829</v>
       </c>
       <c r="AO4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AP4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AQ4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AR4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AS4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AT4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AU4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AV4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AW4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
       <c r="AX4" t="n">
-        <v>3.4401</v>
+        <v>0.3286</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Kun Chaung</t>
+          <t>Phyu Chaung</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>911.9245</v>
+        <v>953.4082</v>
       </c>
       <c r="C5" t="n">
-        <v>625.8341</v>
+        <v>654.3891</v>
       </c>
       <c r="D5" t="n">
-        <v>-45.1733</v>
+        <v>-142.7067</v>
       </c>
       <c r="E5" t="n">
-        <v>286.0904</v>
+        <v>299.0191</v>
       </c>
       <c r="F5" t="n">
-        <v>331.2637</v>
+        <v>441.7258</v>
       </c>
       <c r="G5" t="n">
-        <v>21747.4624</v>
+        <v>18636.4122</v>
       </c>
       <c r="H5" t="n">
-        <v>2174.7462</v>
+        <v>1863.6412</v>
       </c>
       <c r="I5" t="n">
-        <v>2279.953</v>
+        <v>2479.4528</v>
       </c>
       <c r="J5" t="n">
-        <v>1101.2352</v>
+        <v>1246.9535</v>
       </c>
       <c r="K5" t="n">
-        <v>757.3488</v>
+        <v>887.3766000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>483.7747</v>
+        <v>601.3201</v>
       </c>
       <c r="M5" t="n">
-        <v>350.4669</v>
+        <v>461.9298</v>
       </c>
       <c r="N5" t="n">
-        <v>266.1365</v>
+        <v>373.7517</v>
       </c>
       <c r="O5" t="n">
-        <v>206.0211</v>
+        <v>310.8934</v>
       </c>
       <c r="P5" t="n">
-        <v>140.7752</v>
+        <v>242.6706</v>
       </c>
       <c r="Q5" t="n">
-        <v>92.9973</v>
+        <v>192.7127</v>
       </c>
       <c r="R5" t="n">
-        <v>45.1733</v>
+        <v>142.7067</v>
       </c>
       <c r="S5" t="n">
-        <v>236.9741</v>
+        <v>253.3545</v>
       </c>
       <c r="T5" t="n">
-        <v>231.526</v>
+        <v>248.6511</v>
       </c>
       <c r="U5" t="n">
-        <v>609.4919</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>1077.9919</v>
+        <v>502.0057</v>
       </c>
       <c r="X5" t="n">
-        <v>70770.17140000001</v>
+        <v>21179.6186</v>
       </c>
       <c r="Y5" t="n">
-        <v>7077.0171</v>
+        <v>2117.9619</v>
       </c>
       <c r="Z5" t="n">
-        <v>3039.9022</v>
+        <v>1081.5836</v>
       </c>
       <c r="AA5" t="n">
-        <v>2695.8843</v>
+        <v>979.5374</v>
       </c>
       <c r="AB5" t="n">
-        <v>2324.5034</v>
+        <v>869.3769</v>
       </c>
       <c r="AC5" t="n">
-        <v>1741.2096</v>
+        <v>696.3642</v>
       </c>
       <c r="AD5" t="n">
-        <v>1320.4745</v>
+        <v>571.5747</v>
       </c>
       <c r="AE5" t="n">
-        <v>1016.9945</v>
+        <v>481.5674</v>
       </c>
       <c r="AF5" t="n">
-        <v>798.0915</v>
+        <v>416.6475</v>
       </c>
       <c r="AG5" t="n">
-        <v>578.6081</v>
+        <v>351.5593</v>
       </c>
       <c r="AH5" t="n">
-        <v>444.151</v>
+        <v>311.6887</v>
       </c>
       <c r="AI5" t="n">
-        <v>342.152</v>
+        <v>281.4455</v>
       </c>
       <c r="AJ5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AK5" t="n">
-        <v>1.3163</v>
+        <v>1.9079</v>
       </c>
       <c r="AL5" t="n">
-        <v>2.2593</v>
+        <v>2.6906</v>
       </c>
       <c r="AM5" t="n">
-        <v>210.2304</v>
+        <v>146.5408</v>
       </c>
       <c r="AN5" t="n">
-        <v>21.023</v>
+        <v>14.6541</v>
       </c>
       <c r="AO5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AP5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AQ5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AR5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AS5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AT5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AU5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AV5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AW5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
       <c r="AX5" t="n">
-        <v>3.2023</v>
+        <v>3.4734</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Thauk Ye Khat 2</t>
+          <t>Shwegyin</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>783.4004</v>
+        <v>783.8199</v>
       </c>
       <c r="C6" t="n">
-        <v>537.6308</v>
+        <v>537.989</v>
       </c>
       <c r="D6" t="n">
-        <v>-48.2533</v>
+        <v>-116.5267</v>
       </c>
       <c r="E6" t="n">
-        <v>245.7696</v>
+        <v>245.8308</v>
       </c>
       <c r="F6" t="n">
-        <v>294.0229</v>
+        <v>362.3575</v>
       </c>
       <c r="G6" t="n">
-        <v>2531.5373</v>
+        <v>31173.254</v>
       </c>
       <c r="H6" t="n">
-        <v>253.1537</v>
+        <v>3117.3254</v>
       </c>
       <c r="I6" t="n">
-        <v>1968.0693</v>
+        <v>2037.6219</v>
       </c>
       <c r="J6" t="n">
-        <v>955.4767000000001</v>
+        <v>1024.3546</v>
       </c>
       <c r="K6" t="n">
-        <v>660.0568</v>
+        <v>728.7378</v>
       </c>
       <c r="L6" t="n">
-        <v>425.0394</v>
+        <v>493.5638</v>
       </c>
       <c r="M6" t="n">
-        <v>310.5196</v>
+        <v>378.9677</v>
       </c>
       <c r="N6" t="n">
-        <v>238.0745</v>
+        <v>306.4743</v>
       </c>
       <c r="O6" t="n">
-        <v>186.4316</v>
+        <v>254.797</v>
       </c>
       <c r="P6" t="n">
-        <v>130.3814</v>
+        <v>198.7094</v>
       </c>
       <c r="Q6" t="n">
-        <v>89.33710000000001</v>
+        <v>157.6378</v>
       </c>
       <c r="R6" t="n">
-        <v>48.2533</v>
+        <v>116.5267</v>
       </c>
       <c r="S6" t="n">
-        <v>183.9916</v>
+        <v>201.9934</v>
       </c>
       <c r="T6" t="n">
-        <v>134.7671</v>
+        <v>123.2074</v>
       </c>
       <c r="U6" t="n">
-        <v>954.7034</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>1273.4621</v>
+        <v>325.2008</v>
       </c>
       <c r="X6" t="n">
-        <v>10964.5087</v>
+        <v>27976.7012</v>
       </c>
       <c r="Y6" t="n">
-        <v>1096.4509</v>
+        <v>2797.6701</v>
       </c>
       <c r="Z6" t="n">
-        <v>3897.8939</v>
+        <v>787.2843</v>
       </c>
       <c r="AA6" t="n">
-        <v>3436.9328</v>
+        <v>705.9253</v>
       </c>
       <c r="AB6" t="n">
-        <v>2939.3054</v>
+        <v>618.0971</v>
       </c>
       <c r="AC6" t="n">
-        <v>2157.7229</v>
+        <v>480.1582</v>
       </c>
       <c r="AD6" t="n">
-        <v>1593.9556</v>
+        <v>380.6666</v>
       </c>
       <c r="AE6" t="n">
-        <v>1187.3018</v>
+        <v>308.9059</v>
       </c>
       <c r="AF6" t="n">
-        <v>893.9763</v>
+        <v>257.1468</v>
       </c>
       <c r="AG6" t="n">
-        <v>599.8699</v>
+        <v>205.2536</v>
       </c>
       <c r="AH6" t="n">
-        <v>419.696</v>
+        <v>173.4657</v>
       </c>
       <c r="AI6" t="n">
-        <v>283.0143</v>
+        <v>149.3536</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.2595</v>
+        <v>0.2151</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.294</v>
+        <v>0.4117</v>
       </c>
       <c r="AM6" t="n">
-        <v>2.8289</v>
+        <v>52.3262</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.2829</v>
+        <v>5.2326</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AV6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
       <c r="AX6" t="n">
-        <v>0.3286</v>
+        <v>0.6082</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Phyu Chaung</t>
+          <t>Belin</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>953.5329</v>
+        <v>541.4186</v>
       </c>
       <c r="C7" t="n">
-        <v>654.3891</v>
+        <v>371.6125</v>
       </c>
       <c r="D7" t="n">
-        <v>-142.7067</v>
+        <v>-76.4867</v>
       </c>
       <c r="E7" t="n">
-        <v>299.1438</v>
+        <v>169.8061</v>
       </c>
       <c r="F7" t="n">
-        <v>441.8505</v>
+        <v>246.2928</v>
       </c>
       <c r="G7" t="n">
-        <v>18641.6728</v>
+        <v>107103.8525</v>
       </c>
       <c r="H7" t="n">
-        <v>1864.1673</v>
+        <v>10710.3852</v>
       </c>
       <c r="I7" t="n">
-        <v>2479.4528</v>
+        <v>1403.471</v>
       </c>
       <c r="J7" t="n">
-        <v>1246.9535</v>
+        <v>703.563</v>
       </c>
       <c r="K7" t="n">
-        <v>887.3766000000001</v>
+        <v>499.3676</v>
       </c>
       <c r="L7" t="n">
-        <v>601.3201</v>
+        <v>336.9227</v>
       </c>
       <c r="M7" t="n">
-        <v>461.9298</v>
+        <v>257.7662</v>
       </c>
       <c r="N7" t="n">
-        <v>373.7517</v>
+        <v>207.6918</v>
       </c>
       <c r="O7" t="n">
-        <v>310.8934</v>
+        <v>171.996</v>
       </c>
       <c r="P7" t="n">
-        <v>242.6706</v>
+        <v>133.2539</v>
       </c>
       <c r="Q7" t="n">
-        <v>192.7127</v>
+        <v>104.884</v>
       </c>
       <c r="R7" t="n">
-        <v>142.7067</v>
+        <v>76.4867</v>
       </c>
       <c r="S7" t="n">
-        <v>245.2103</v>
+        <v>112.7692</v>
       </c>
       <c r="T7" t="n">
-        <v>248.6511</v>
+        <v>42.5642</v>
       </c>
       <c r="U7" t="n">
-        <v>799.3289</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>1293.1903</v>
+        <v>155.3334</v>
       </c>
       <c r="X7" t="n">
-        <v>54559.7004</v>
+        <v>67548.8864</v>
       </c>
       <c r="Y7" t="n">
-        <v>5455.97</v>
+        <v>6754.8886</v>
       </c>
       <c r="Z7" t="n">
-        <v>3709.005</v>
+        <v>413.306</v>
       </c>
       <c r="AA7" t="n">
-        <v>3285.1255</v>
+        <v>367.8848</v>
       </c>
       <c r="AB7" t="n">
-        <v>2827.5304</v>
+        <v>318.8519</v>
       </c>
       <c r="AC7" t="n">
-        <v>2108.8261</v>
+        <v>241.8432</v>
       </c>
       <c r="AD7" t="n">
-        <v>1590.4165</v>
+        <v>186.2989</v>
       </c>
       <c r="AE7" t="n">
-        <v>1216.4817</v>
+        <v>146.2362</v>
       </c>
       <c r="AF7" t="n">
-        <v>946.7583</v>
+        <v>117.3401</v>
       </c>
       <c r="AG7" t="n">
-        <v>676.3187</v>
+        <v>88.369</v>
       </c>
       <c r="AH7" t="n">
-        <v>510.6446</v>
+        <v>70.6225</v>
       </c>
       <c r="AI7" t="n">
-        <v>384.9637</v>
+        <v>57.1611</v>
       </c>
       <c r="AJ7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AK7" t="n">
-        <v>1.9079</v>
+        <v>0.1043</v>
       </c>
       <c r="AL7" t="n">
-        <v>2.6906</v>
+        <v>0.3058</v>
       </c>
       <c r="AM7" t="n">
-        <v>146.5408</v>
+        <v>220.6093</v>
       </c>
       <c r="AN7" t="n">
-        <v>14.6541</v>
+        <v>22.0609</v>
       </c>
       <c r="AO7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AP7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AQ7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AR7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AS7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AT7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AU7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AV7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AW7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
       <c r="AX7" t="n">
-        <v>3.4734</v>
+        <v>0.5073</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Shwegyin</t>
+          <t>Yunzalin</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>783.9224</v>
+        <v>614.0088</v>
       </c>
       <c r="C8" t="n">
-        <v>537.989</v>
+        <v>421.4361</v>
       </c>
       <c r="D8" t="n">
-        <v>-116.5267</v>
+        <v>-15.4</v>
       </c>
       <c r="E8" t="n">
-        <v>245.9334</v>
+        <v>192.5727</v>
       </c>
       <c r="F8" t="n">
-        <v>362.46</v>
+        <v>207.9727</v>
       </c>
       <c r="G8" t="n">
-        <v>31182.0729</v>
+        <v>1412.3425</v>
       </c>
       <c r="H8" t="n">
-        <v>3118.2073</v>
+        <v>141.2343</v>
       </c>
       <c r="I8" t="n">
-        <v>2037.6219</v>
+        <v>1520.2986</v>
       </c>
       <c r="J8" t="n">
-        <v>1024.3546</v>
+        <v>726.5511</v>
       </c>
       <c r="K8" t="n">
-        <v>728.7378</v>
+        <v>494.9783</v>
       </c>
       <c r="L8" t="n">
-        <v>493.5638</v>
+        <v>310.7537</v>
       </c>
       <c r="M8" t="n">
-        <v>378.9677</v>
+        <v>220.9844</v>
       </c>
       <c r="N8" t="n">
-        <v>306.4743</v>
+        <v>164.1964</v>
       </c>
       <c r="O8" t="n">
-        <v>254.797</v>
+        <v>123.7147</v>
       </c>
       <c r="P8" t="n">
-        <v>198.7094</v>
+        <v>79.7782</v>
       </c>
       <c r="Q8" t="n">
-        <v>157.6378</v>
+        <v>47.6046</v>
       </c>
       <c r="R8" t="n">
-        <v>116.5267</v>
+        <v>15.4</v>
       </c>
       <c r="S8" t="n">
-        <v>195.5002</v>
+        <v>103.0448</v>
       </c>
       <c r="T8" t="n">
-        <v>123.2074</v>
+        <v>44.8219</v>
       </c>
       <c r="U8" t="n">
-        <v>506.5099</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>825.2175</v>
+        <v>147.8667</v>
       </c>
       <c r="X8" t="n">
-        <v>70992.63430000001</v>
+        <v>1004.1628</v>
       </c>
       <c r="Y8" t="n">
-        <v>7099.2634</v>
+        <v>100.4163</v>
       </c>
       <c r="Z8" t="n">
-        <v>2452.1995</v>
+        <v>383.5937</v>
       </c>
       <c r="AA8" t="n">
-        <v>2166.9048</v>
+        <v>342.0893</v>
       </c>
       <c r="AB8" t="n">
-        <v>1858.918</v>
+        <v>297.2846</v>
       </c>
       <c r="AC8" t="n">
-        <v>1375.1913</v>
+        <v>226.9166</v>
       </c>
       <c r="AD8" t="n">
-        <v>1026.2749</v>
+        <v>176.162</v>
       </c>
       <c r="AE8" t="n">
-        <v>774.5982</v>
+        <v>139.554</v>
       </c>
       <c r="AF8" t="n">
-        <v>593.0616</v>
+        <v>113.1497</v>
       </c>
       <c r="AG8" t="n">
-        <v>411.0435</v>
+        <v>86.6769</v>
       </c>
       <c r="AH8" t="n">
-        <v>299.5379</v>
+        <v>70.4607</v>
       </c>
       <c r="AI8" t="n">
-        <v>214.9498</v>
+        <v>58.1601</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.2151</v>
+        <v>1.6008</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.4117</v>
+        <v>2.2033</v>
       </c>
       <c r="AM8" t="n">
-        <v>52.3262</v>
+        <v>19.0548</v>
       </c>
       <c r="AN8" t="n">
-        <v>5.2326</v>
+        <v>1.9055</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AQ8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AS8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AW8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.6082</v>
+        <v>2.8059</v>
       </c>
     </row>
     <row r="9">
@@ -5155,7 +5155,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>755.0835</v>
+        <v>754.9848</v>
       </c>
       <c r="C9" t="n">
         <v>518.1975</v>
@@ -5164,16 +5164,16 @@
         <v>-224.84</v>
       </c>
       <c r="E9" t="n">
-        <v>236.886</v>
+        <v>236.7872</v>
       </c>
       <c r="F9" t="n">
-        <v>461.726</v>
+        <v>461.6272</v>
       </c>
       <c r="G9" t="n">
-        <v>13714.1852</v>
+        <v>13711.2524</v>
       </c>
       <c r="H9" t="n">
-        <v>1371.4185</v>
+        <v>1371.1252</v>
       </c>
       <c r="I9" t="n">
         <v>2075.2622</v>
@@ -5206,55 +5206,55 @@
         <v>224.84</v>
       </c>
       <c r="S9" t="n">
-        <v>126.934</v>
+        <v>131.1499</v>
       </c>
       <c r="T9" t="n">
         <v>87.55289999999999</v>
       </c>
       <c r="U9" t="n">
-        <v>272.1178</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>486.6047</v>
+        <v>218.7028</v>
       </c>
       <c r="X9" t="n">
-        <v>14453.1317</v>
+        <v>6495.9096</v>
       </c>
       <c r="Y9" t="n">
-        <v>1445.3132</v>
+        <v>649.591</v>
       </c>
       <c r="Z9" t="n">
-        <v>1413.1838</v>
+        <v>518.7234</v>
       </c>
       <c r="AA9" t="n">
-        <v>1250.7966</v>
+        <v>465.8988</v>
       </c>
       <c r="AB9" t="n">
-        <v>1075.4935</v>
+        <v>408.8738</v>
       </c>
       <c r="AC9" t="n">
-        <v>800.1615</v>
+        <v>319.3132</v>
       </c>
       <c r="AD9" t="n">
-        <v>601.5626</v>
+        <v>254.7155</v>
       </c>
       <c r="AE9" t="n">
-        <v>458.3118</v>
+        <v>208.1228</v>
       </c>
       <c r="AF9" t="n">
-        <v>354.9839</v>
+        <v>174.5168</v>
       </c>
       <c r="AG9" t="n">
-        <v>251.3824</v>
+        <v>140.8237</v>
       </c>
       <c r="AH9" t="n">
-        <v>187.9156</v>
+        <v>120.1845</v>
       </c>
       <c r="AI9" t="n">
-        <v>139.77</v>
+        <v>104.529</v>
       </c>
       <c r="AJ9" t="n">
         <v>0.5632</v>
@@ -5309,7 +5309,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>877.6264</v>
+        <v>877.5117</v>
       </c>
       <c r="C10" t="n">
         <v>602.2961</v>
@@ -5318,16 +5318,16 @@
         <v>-26.6933</v>
       </c>
       <c r="E10" t="n">
-        <v>275.3303</v>
+        <v>275.2156</v>
       </c>
       <c r="F10" t="n">
-        <v>302.0237</v>
+        <v>301.9089</v>
       </c>
       <c r="G10" t="n">
-        <v>23026.8889</v>
+        <v>23018.139</v>
       </c>
       <c r="H10" t="n">
-        <v>2302.6889</v>
+        <v>2301.8139</v>
       </c>
       <c r="I10" t="n">
         <v>2177.4216</v>
@@ -5360,55 +5360,55 @@
         <v>26.6933</v>
       </c>
       <c r="S10" t="n">
-        <v>236.9001</v>
+        <v>244.7683</v>
       </c>
       <c r="T10" t="n">
         <v>215.7673</v>
       </c>
       <c r="U10" t="n">
-        <v>704.432</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
         <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>1157.0994</v>
+        <v>460.5356</v>
       </c>
       <c r="X10" t="n">
-        <v>88219.5742</v>
+        <v>35112.1588</v>
       </c>
       <c r="Y10" t="n">
-        <v>8821.957399999999</v>
+        <v>3511.2159</v>
       </c>
       <c r="Z10" t="n">
-        <v>3335.9637</v>
+        <v>1020.4717</v>
       </c>
       <c r="AA10" t="n">
-        <v>2953.7509</v>
+        <v>921.8838</v>
       </c>
       <c r="AB10" t="n">
-        <v>2541.1368</v>
+        <v>815.4567</v>
       </c>
       <c r="AC10" t="n">
-        <v>1893.0808</v>
+        <v>648.3074</v>
       </c>
       <c r="AD10" t="n">
-        <v>1425.6311</v>
+        <v>527.747</v>
       </c>
       <c r="AE10" t="n">
-        <v>1088.4548</v>
+        <v>440.79</v>
       </c>
       <c r="AF10" t="n">
-        <v>845.246</v>
+        <v>378.0702</v>
       </c>
       <c r="AG10" t="n">
-        <v>601.3916</v>
+        <v>315.1879</v>
       </c>
       <c r="AH10" t="n">
-        <v>452.0042</v>
+        <v>276.6686</v>
       </c>
       <c r="AI10" t="n">
-        <v>338.6788</v>
+        <v>247.4503</v>
       </c>
       <c r="AJ10" t="n">
         <v>3.2198</v>
@@ -5463,7 +5463,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>423.7947</v>
+        <v>423.7393</v>
       </c>
       <c r="C11" t="n">
         <v>290.8412</v>
@@ -5472,16 +5472,16 @@
         <v>-10.4133</v>
       </c>
       <c r="E11" t="n">
-        <v>132.9535</v>
+        <v>132.8981</v>
       </c>
       <c r="F11" t="n">
-        <v>143.3669</v>
+        <v>143.3115</v>
       </c>
       <c r="G11" t="n">
-        <v>3899.8657</v>
+        <v>3898.3582</v>
       </c>
       <c r="H11" t="n">
-        <v>389.9866</v>
+        <v>389.8358</v>
       </c>
       <c r="I11" t="n">
         <v>1048.9728</v>
@@ -5514,55 +5514,55 @@
         <v>10.4133</v>
       </c>
       <c r="S11" t="n">
-        <v>228.8881</v>
+        <v>236.4902</v>
       </c>
       <c r="T11" t="n">
         <v>168.8782</v>
       </c>
       <c r="U11" t="n">
-        <v>5538.9185</v>
+        <v>0</v>
       </c>
       <c r="V11" t="n">
         <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>5936.6848</v>
+        <v>405.3684</v>
       </c>
       <c r="X11" t="n">
-        <v>161489.6986</v>
+        <v>11026.8313</v>
       </c>
       <c r="Y11" t="n">
-        <v>16148.9699</v>
+        <v>1102.6831</v>
       </c>
       <c r="Z11" t="n">
-        <v>19152.9806</v>
+        <v>946.3673</v>
       </c>
       <c r="AA11" t="n">
-        <v>16827.5962</v>
+        <v>851.1137</v>
       </c>
       <c r="AB11" t="n">
-        <v>14317.2336</v>
+        <v>748.2859</v>
       </c>
       <c r="AC11" t="n">
-        <v>10374.3887</v>
+        <v>586.7897</v>
       </c>
       <c r="AD11" t="n">
-        <v>7530.3305</v>
+        <v>470.3067</v>
       </c>
       <c r="AE11" t="n">
-        <v>5478.8507</v>
+        <v>386.2906</v>
       </c>
       <c r="AF11" t="n">
-        <v>3999.0746</v>
+        <v>325.692</v>
       </c>
       <c r="AG11" t="n">
-        <v>2515.3439</v>
+        <v>264.9364</v>
       </c>
       <c r="AH11" t="n">
-        <v>1606.3766</v>
+        <v>227.7198</v>
       </c>
       <c r="AI11" t="n">
-        <v>916.8150000000001</v>
+        <v>199.4897</v>
       </c>
       <c r="AJ11" t="n">
         <v>0.06</v>
@@ -5617,7 +5617,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>554.2396</v>
+        <v>554.1671</v>
       </c>
       <c r="C12" t="n">
         <v>380.3627</v>
@@ -5626,16 +5626,16 @@
         <v>-498.96</v>
       </c>
       <c r="E12" t="n">
-        <v>173.8769</v>
+        <v>173.8044</v>
       </c>
       <c r="F12" t="n">
-        <v>672.8369</v>
+        <v>672.7644</v>
       </c>
       <c r="G12" t="n">
-        <v>6759.3197</v>
+        <v>6758.5916</v>
       </c>
       <c r="H12" t="n">
-        <v>675.932</v>
+        <v>675.8592</v>
       </c>
       <c r="I12" t="n">
         <v>1857.1903</v>
@@ -5668,55 +5668,55 @@
         <v>498.96</v>
       </c>
       <c r="S12" t="n">
-        <v>84.8171</v>
+        <v>87.63420000000001</v>
       </c>
       <c r="T12" t="n">
         <v>41.5745</v>
       </c>
       <c r="U12" t="n">
-        <v>118.1406</v>
+        <v>0</v>
       </c>
       <c r="V12" t="n">
         <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>244.5322</v>
+        <v>129.2086</v>
       </c>
       <c r="X12" t="n">
-        <v>2456.5706</v>
+        <v>1298.0301</v>
       </c>
       <c r="Y12" t="n">
-        <v>245.6571</v>
+        <v>129.803</v>
       </c>
       <c r="Z12" t="n">
-        <v>718.0142</v>
+        <v>329.682</v>
       </c>
       <c r="AA12" t="n">
-        <v>635.15</v>
+        <v>294.3847</v>
       </c>
       <c r="AB12" t="n">
-        <v>545.6953</v>
+        <v>256.2807</v>
       </c>
       <c r="AC12" t="n">
-        <v>405.1979</v>
+        <v>196.4364</v>
       </c>
       <c r="AD12" t="n">
-        <v>303.8568</v>
+        <v>153.2723</v>
       </c>
       <c r="AE12" t="n">
-        <v>230.7593</v>
+        <v>122.1391</v>
       </c>
       <c r="AF12" t="n">
-        <v>178.0339</v>
+        <v>99.6836</v>
       </c>
       <c r="AG12" t="n">
-        <v>125.1693</v>
+        <v>77.1699</v>
       </c>
       <c r="AH12" t="n">
-        <v>92.78449999999999</v>
+        <v>63.3789</v>
       </c>
       <c r="AI12" t="n">
-        <v>68.2179</v>
+        <v>52.9179</v>
       </c>
       <c r="AJ12" t="n">
         <v>2.3092</v>
@@ -5878,74 +5878,74 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Yunzalin</t>
+          <t>Kabaung</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>38.3392</v>
+        <v>198.1951</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3653</v>
+        <v>0.4606</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>eutrophic</t>
+          <t>hyper eutrophic</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>17.5786</v>
+        <v>113.3709</v>
       </c>
       <c r="F2" t="n">
-        <v>11.1568</v>
+        <v>61.0773</v>
       </c>
       <c r="G2" t="n">
-        <v>24.2825</v>
+        <v>110.0399</v>
       </c>
       <c r="H2" t="n">
-        <v>2.7738</v>
+        <v>14.1799</v>
       </c>
       <c r="I2" t="n">
-        <v>4.92</v>
+        <v>5.03</v>
       </c>
       <c r="J2" t="n">
-        <v>59.04</v>
+        <v>60.36</v>
       </c>
       <c r="K2" t="n">
-        <v>24.6835</v>
+        <v>24.8804</v>
       </c>
       <c r="L2" t="n">
-        <v>997.1558</v>
+        <v>997.1057</v>
       </c>
       <c r="M2" t="n">
-        <v>27.425</v>
+        <v>28.475</v>
       </c>
       <c r="N2" t="n">
-        <v>996.4261</v>
+        <v>996.1283</v>
       </c>
       <c r="O2" t="n">
-        <v>1.459</v>
+        <v>2.0544</v>
       </c>
       <c r="P2" t="n">
-        <v>11297.8458</v>
+        <v>62948.9266</v>
       </c>
       <c r="Q2" t="n">
-        <v>24640.7573</v>
+        <v>110047.3674</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0162</v>
+        <v>0.0827</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Belin</t>
+          <t>Kun Chaung</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15.5957</v>
+        <v>90.0992</v>
       </c>
       <c r="C3" t="n">
-        <v>0.874</v>
+        <v>0.479</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -5953,76 +5953,76 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>14.1373</v>
+        <v>112.5835</v>
       </c>
       <c r="F3" t="n">
-        <v>1.7498</v>
+        <v>57.8858</v>
       </c>
       <c r="G3" t="n">
-        <v>1.9941</v>
+        <v>49.9667</v>
       </c>
       <c r="H3" t="n">
-        <v>2.8402</v>
+        <v>15.8479</v>
       </c>
       <c r="I3" t="n">
-        <v>4.87</v>
+        <v>5.03</v>
       </c>
       <c r="J3" t="n">
-        <v>58.44</v>
+        <v>60.36</v>
       </c>
       <c r="K3" t="n">
-        <v>25.34</v>
+        <v>24.8804</v>
       </c>
       <c r="L3" t="n">
-        <v>996.9874</v>
+        <v>997.1057</v>
       </c>
       <c r="M3" t="n">
-        <v>28.125</v>
+        <v>28.175</v>
       </c>
       <c r="N3" t="n">
-        <v>996.2286</v>
+        <v>996.2144</v>
       </c>
       <c r="O3" t="n">
-        <v>4.0815</v>
+        <v>2.2812</v>
       </c>
       <c r="P3" t="n">
-        <v>42532.0938</v>
+        <v>81706.5491</v>
       </c>
       <c r="Q3" t="n">
-        <v>46919.644</v>
+        <v>65388.7674</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0021</v>
+        <v>0.0776</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Kabaung</t>
+          <t>Thauk Ye Khat 2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>198.1951</v>
+        <v>73.5153</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4606</v>
+        <v>0.1248</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>hyper eutrophic</t>
+          <t>eutrophic</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>113.3709</v>
+        <v>6.8166</v>
       </c>
       <c r="F4" t="n">
-        <v>61.0773</v>
+        <v>5.9489</v>
       </c>
       <c r="G4" t="n">
-        <v>110.0399</v>
+        <v>64.4008</v>
       </c>
       <c r="H4" t="n">
-        <v>14.1799</v>
+        <v>8.394</v>
       </c>
       <c r="I4" t="n">
         <v>5.03</v>
@@ -6031,41 +6031,41 @@
         <v>60.36</v>
       </c>
       <c r="K4" t="n">
-        <v>24.8804</v>
+        <v>25.0773</v>
       </c>
       <c r="L4" t="n">
-        <v>997.1057</v>
+        <v>997.0553</v>
       </c>
       <c r="M4" t="n">
-        <v>28.475</v>
+        <v>28.575</v>
       </c>
       <c r="N4" t="n">
-        <v>996.1283</v>
+        <v>996.0993999999999</v>
       </c>
       <c r="O4" t="n">
-        <v>1.9326</v>
+        <v>1.449</v>
       </c>
       <c r="P4" t="n">
-        <v>62948.9266</v>
+        <v>6582.6157</v>
       </c>
       <c r="Q4" t="n">
-        <v>110047.3674</v>
+        <v>70991.83560000001</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0827</v>
+        <v>0.0086</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Kun Chaung</t>
+          <t>Phyu Chaung</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>90.0992</v>
+        <v>121.1633</v>
       </c>
       <c r="C5" t="n">
-        <v>0.479</v>
+        <v>0.3805</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6073,16 +6073,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>112.5835</v>
+        <v>116.0216</v>
       </c>
       <c r="F5" t="n">
-        <v>57.8858</v>
+        <v>71.7252</v>
       </c>
       <c r="G5" t="n">
-        <v>49.9667</v>
+        <v>77.742</v>
       </c>
       <c r="H5" t="n">
-        <v>15.8479</v>
+        <v>17.2333</v>
       </c>
       <c r="I5" t="n">
         <v>5.03</v>
@@ -6091,41 +6091,41 @@
         <v>60.36</v>
       </c>
       <c r="K5" t="n">
-        <v>24.8804</v>
+        <v>24.6835</v>
       </c>
       <c r="L5" t="n">
-        <v>997.1057</v>
+        <v>997.1558</v>
       </c>
       <c r="M5" t="n">
-        <v>28.175</v>
+        <v>28.2</v>
       </c>
       <c r="N5" t="n">
-        <v>996.2144</v>
+        <v>996.2071999999999</v>
       </c>
       <c r="O5" t="n">
-        <v>2.146</v>
+        <v>2.0417</v>
       </c>
       <c r="P5" t="n">
-        <v>81706.5491</v>
+        <v>81804.50350000001</v>
       </c>
       <c r="Q5" t="n">
-        <v>65388.7674</v>
+        <v>85429.83409999999</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0776</v>
+        <v>0.1034</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Thauk Ye Khat 2</t>
+          <t>Shwegyin</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>73.5153</v>
+        <v>29.9221</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1248</v>
+        <v>0.5264</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -6133,59 +6133,59 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6.8166</v>
+        <v>13.974</v>
       </c>
       <c r="F6" t="n">
-        <v>5.9489</v>
+        <v>6.4728</v>
       </c>
       <c r="G6" t="n">
-        <v>64.4008</v>
+        <v>15.1562</v>
       </c>
       <c r="H6" t="n">
-        <v>8.394</v>
+        <v>8.7935</v>
       </c>
       <c r="I6" t="n">
-        <v>5.03</v>
+        <v>4.94</v>
       </c>
       <c r="J6" t="n">
-        <v>60.36</v>
+        <v>59.28</v>
       </c>
       <c r="K6" t="n">
-        <v>25.0773</v>
+        <v>25.7338</v>
       </c>
       <c r="L6" t="n">
-        <v>997.0553</v>
+        <v>996.8845</v>
       </c>
       <c r="M6" t="n">
-        <v>28.575</v>
+        <v>28.75</v>
       </c>
       <c r="N6" t="n">
-        <v>996.0993999999999</v>
+        <v>996.0486</v>
       </c>
       <c r="O6" t="n">
-        <v>1.3631</v>
+        <v>2.4656</v>
       </c>
       <c r="P6" t="n">
-        <v>6582.6157</v>
+        <v>17381.6019</v>
       </c>
       <c r="Q6" t="n">
-        <v>70991.83560000001</v>
+        <v>37218.7034</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0086</v>
+        <v>0.0081</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Phyu Chaung</t>
+          <t>Belin</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>121.1633</v>
+        <v>15.5957</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3805</v>
+        <v>0.874</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -6193,59 +6193,59 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>116.0216</v>
+        <v>14.1373</v>
       </c>
       <c r="F7" t="n">
-        <v>71.7252</v>
+        <v>1.7498</v>
       </c>
       <c r="G7" t="n">
-        <v>77.742</v>
+        <v>1.9941</v>
       </c>
       <c r="H7" t="n">
-        <v>17.2333</v>
+        <v>2.8402</v>
       </c>
       <c r="I7" t="n">
-        <v>5.03</v>
+        <v>4.87</v>
       </c>
       <c r="J7" t="n">
-        <v>60.36</v>
+        <v>58.44</v>
       </c>
       <c r="K7" t="n">
-        <v>24.6835</v>
+        <v>25.34</v>
       </c>
       <c r="L7" t="n">
-        <v>997.1558</v>
+        <v>996.9874</v>
       </c>
       <c r="M7" t="n">
-        <v>28.2</v>
+        <v>28.125</v>
       </c>
       <c r="N7" t="n">
-        <v>996.2071999999999</v>
+        <v>996.2286</v>
       </c>
       <c r="O7" t="n">
-        <v>1.9207</v>
+        <v>4.3386</v>
       </c>
       <c r="P7" t="n">
-        <v>81804.50350000001</v>
+        <v>42532.0938</v>
       </c>
       <c r="Q7" t="n">
-        <v>85429.83409999999</v>
+        <v>46919.644</v>
       </c>
       <c r="R7" t="n">
-        <v>0.1034</v>
+        <v>0.0021</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Shwegyin</t>
+          <t>Yunzalin</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>29.9221</v>
+        <v>38.3392</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5264</v>
+        <v>0.3653</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -6253,46 +6253,46 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>13.974</v>
+        <v>17.5786</v>
       </c>
       <c r="F8" t="n">
-        <v>6.4728</v>
+        <v>11.1568</v>
       </c>
       <c r="G8" t="n">
-        <v>15.1562</v>
+        <v>24.2825</v>
       </c>
       <c r="H8" t="n">
-        <v>8.7935</v>
+        <v>2.7738</v>
       </c>
       <c r="I8" t="n">
-        <v>4.94</v>
+        <v>4.92</v>
       </c>
       <c r="J8" t="n">
-        <v>59.28</v>
+        <v>59.04</v>
       </c>
       <c r="K8" t="n">
-        <v>25.7338</v>
+        <v>24.6835</v>
       </c>
       <c r="L8" t="n">
-        <v>996.8845</v>
+        <v>997.1558</v>
       </c>
       <c r="M8" t="n">
-        <v>28.75</v>
+        <v>27.425</v>
       </c>
       <c r="N8" t="n">
-        <v>996.0486</v>
+        <v>996.4261</v>
       </c>
       <c r="O8" t="n">
-        <v>2.3194</v>
+        <v>1.5509</v>
       </c>
       <c r="P8" t="n">
-        <v>17381.6019</v>
+        <v>11297.8458</v>
       </c>
       <c r="Q8" t="n">
-        <v>37218.7034</v>
+        <v>24640.7573</v>
       </c>
       <c r="R8" t="n">
-        <v>0.0081</v>
+        <v>0.0162</v>
       </c>
     </row>
     <row r="9">
@@ -6343,7 +6343,7 @@
         <v>996.3561</v>
       </c>
       <c r="O9" t="n">
-        <v>2.1024</v>
+        <v>2.2349</v>
       </c>
       <c r="P9" t="n">
         <v>4314.405</v>
@@ -6403,7 +6403,7 @@
         <v>996.1283</v>
       </c>
       <c r="O10" t="n">
-        <v>2.1756</v>
+        <v>2.3127</v>
       </c>
       <c r="P10" t="n">
         <v>101292.0643</v>
@@ -6463,7 +6463,7 @@
         <v>996.2071999999999</v>
       </c>
       <c r="O11" t="n">
-        <v>1.7829</v>
+        <v>1.8952</v>
       </c>
       <c r="P11" t="n">
         <v>217901.8936</v>
@@ -6523,7 +6523,7 @@
         <v>996.5368999999999</v>
       </c>
       <c r="O12" t="n">
-        <v>1.6092</v>
+        <v>1.7106</v>
       </c>
       <c r="P12" t="n">
         <v>4560.3566</v>

</xml_diff>